<commit_message>
added Email report to unittest
</commit_message>
<xml_diff>
--- a/Week_2/XConvertor/test/generated_file_by_testing/x_convertor.xlsx
+++ b/Week_2/XConvertor/test/generated_file_by_testing/x_convertor.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CU41"/>
+  <dimension ref="A1:CT41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -871,60 +871,55 @@
       </c>
       <c r="CJ1" s="1" t="inlineStr">
         <is>
+          <t>measurements_1_elementMeasurements_Diameter</t>
+        </is>
+      </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
           <t>measurements_1_elementMeasurements_Height</t>
         </is>
       </c>
-      <c r="CK1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
+        <is>
+          <t>measurements_1_elementMeasurements_Weight</t>
+        </is>
+      </c>
+      <c r="CM1" s="1" t="inlineStr">
         <is>
           <t>measurements_2_elementName</t>
         </is>
       </c>
-      <c r="CL1" s="1" t="inlineStr">
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>measurements_2_elementDescription</t>
         </is>
       </c>
-      <c r="CM1" s="1" t="inlineStr">
-        <is>
-          <t>measurements_2_elementMeasurements_Depth</t>
-        </is>
-      </c>
-      <c r="CN1" s="1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>measurements_2_elementMeasurements_Height</t>
         </is>
       </c>
-      <c r="CO1" s="1" t="inlineStr">
-        <is>
-          <t>measurements_2_elementMeasurements_Weight</t>
-        </is>
-      </c>
       <c r="CP1" s="1" t="inlineStr">
         <is>
-          <t>measurements_2_elementMeasurements_Width</t>
+          <t>tags_3_term</t>
         </is>
       </c>
       <c r="CQ1" s="1" t="inlineStr">
         <is>
-          <t>tags_3_term</t>
+          <t>tags_3_AAT_URL</t>
         </is>
       </c>
       <c r="CR1" s="1" t="inlineStr">
         <is>
-          <t>tags_3_AAT_URL</t>
+          <t>tags_3_Wikidata_URL</t>
         </is>
       </c>
       <c r="CS1" s="1" t="inlineStr">
         <is>
-          <t>tags_3_Wikidata_URL</t>
+          <t>additionalImages_0</t>
         </is>
       </c>
       <c r="CT1" s="1" t="inlineStr">
-        <is>
-          <t>additionalImages_0</t>
-        </is>
-      </c>
-      <c r="CU1" s="1" t="inlineStr">
         <is>
           <t>additionalImages_1</t>
         </is>
@@ -1147,7 +1142,6 @@
       <c r="CR2" t="inlineStr"/>
       <c r="CS2" t="inlineStr"/>
       <c r="CT2" t="inlineStr"/>
-      <c r="CU2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1362,7 +1356,6 @@
       <c r="CR3" t="inlineStr"/>
       <c r="CS3" t="inlineStr"/>
       <c r="CT3" t="inlineStr"/>
-      <c r="CU3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1537,7 +1530,6 @@
       <c r="CR4" t="inlineStr"/>
       <c r="CS4" t="inlineStr"/>
       <c r="CT4" t="inlineStr"/>
-      <c r="CU4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1712,7 +1704,6 @@
       <c r="CR5" t="inlineStr"/>
       <c r="CS5" t="inlineStr"/>
       <c r="CT5" t="inlineStr"/>
-      <c r="CU5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1887,7 +1878,6 @@
       <c r="CR6" t="inlineStr"/>
       <c r="CS6" t="inlineStr"/>
       <c r="CT6" t="inlineStr"/>
-      <c r="CU6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -2062,7 +2052,6 @@
       <c r="CR7" t="inlineStr"/>
       <c r="CS7" t="inlineStr"/>
       <c r="CT7" t="inlineStr"/>
-      <c r="CU7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -2261,7 +2250,6 @@
       <c r="CR8" t="inlineStr"/>
       <c r="CS8" t="inlineStr"/>
       <c r="CT8" t="inlineStr"/>
-      <c r="CU8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -2472,7 +2460,6 @@
       <c r="CR9" t="inlineStr"/>
       <c r="CS9" t="inlineStr"/>
       <c r="CT9" t="inlineStr"/>
-      <c r="CU9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -2647,7 +2634,6 @@
       <c r="CR10" t="inlineStr"/>
       <c r="CS10" t="inlineStr"/>
       <c r="CT10" t="inlineStr"/>
-      <c r="CU10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -2872,7 +2858,6 @@
       <c r="CR11" t="inlineStr"/>
       <c r="CS11" t="inlineStr"/>
       <c r="CT11" t="inlineStr"/>
-      <c r="CU11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -3097,7 +3082,6 @@
       <c r="CR12" t="inlineStr"/>
       <c r="CS12" t="inlineStr"/>
       <c r="CT12" t="inlineStr"/>
-      <c r="CU12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -3326,7 +3310,6 @@
       <c r="CR13" t="inlineStr"/>
       <c r="CS13" t="inlineStr"/>
       <c r="CT13" t="inlineStr"/>
-      <c r="CU13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -3551,7 +3534,6 @@
       <c r="CR14" t="inlineStr"/>
       <c r="CS14" t="inlineStr"/>
       <c r="CT14" t="inlineStr"/>
-      <c r="CU14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -3776,7 +3758,6 @@
       <c r="CR15" t="inlineStr"/>
       <c r="CS15" t="inlineStr"/>
       <c r="CT15" t="inlineStr"/>
-      <c r="CU15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -3963,7 +3944,6 @@
       <c r="CR16" t="inlineStr"/>
       <c r="CS16" t="inlineStr"/>
       <c r="CT16" t="inlineStr"/>
-      <c r="CU16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -4150,7 +4130,6 @@
       <c r="CR17" t="inlineStr"/>
       <c r="CS17" t="inlineStr"/>
       <c r="CT17" t="inlineStr"/>
-      <c r="CU17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -4337,7 +4316,6 @@
       <c r="CR18" t="inlineStr"/>
       <c r="CS18" t="inlineStr"/>
       <c r="CT18" t="inlineStr"/>
-      <c r="CU18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -4524,7 +4502,6 @@
       <c r="CR19" t="inlineStr"/>
       <c r="CS19" t="inlineStr"/>
       <c r="CT19" t="inlineStr"/>
-      <c r="CU19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -4711,7 +4688,6 @@
       <c r="CR20" t="inlineStr"/>
       <c r="CS20" t="inlineStr"/>
       <c r="CT20" t="inlineStr"/>
-      <c r="CU20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -4898,7 +4874,6 @@
       <c r="CR21" t="inlineStr"/>
       <c r="CS21" t="inlineStr"/>
       <c r="CT21" t="inlineStr"/>
-      <c r="CU21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -5085,7 +5060,6 @@
       <c r="CR22" t="inlineStr"/>
       <c r="CS22" t="inlineStr"/>
       <c r="CT22" t="inlineStr"/>
-      <c r="CU22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -5272,7 +5246,6 @@
       <c r="CR23" t="inlineStr"/>
       <c r="CS23" t="inlineStr"/>
       <c r="CT23" t="inlineStr"/>
-      <c r="CU23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -5459,7 +5432,6 @@
       <c r="CR24" t="inlineStr"/>
       <c r="CS24" t="inlineStr"/>
       <c r="CT24" t="inlineStr"/>
-      <c r="CU24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -5646,7 +5618,6 @@
       <c r="CR25" t="inlineStr"/>
       <c r="CS25" t="inlineStr"/>
       <c r="CT25" t="inlineStr"/>
-      <c r="CU25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -5833,7 +5804,6 @@
       <c r="CR26" t="inlineStr"/>
       <c r="CS26" t="inlineStr"/>
       <c r="CT26" t="inlineStr"/>
-      <c r="CU26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -6020,7 +5990,6 @@
       <c r="CR27" t="inlineStr"/>
       <c r="CS27" t="inlineStr"/>
       <c r="CT27" t="inlineStr"/>
-      <c r="CU27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -6207,7 +6176,6 @@
       <c r="CR28" t="inlineStr"/>
       <c r="CS28" t="inlineStr"/>
       <c r="CT28" t="inlineStr"/>
-      <c r="CU28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -6394,7 +6362,6 @@
       <c r="CR29" t="inlineStr"/>
       <c r="CS29" t="inlineStr"/>
       <c r="CT29" t="inlineStr"/>
-      <c r="CU29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -6581,7 +6548,6 @@
       <c r="CR30" t="inlineStr"/>
       <c r="CS30" t="inlineStr"/>
       <c r="CT30" t="inlineStr"/>
-      <c r="CU30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -6768,7 +6734,6 @@
       <c r="CR31" t="inlineStr"/>
       <c r="CS31" t="inlineStr"/>
       <c r="CT31" t="inlineStr"/>
-      <c r="CU31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -6955,7 +6920,6 @@
       <c r="CR32" t="inlineStr"/>
       <c r="CS32" t="inlineStr"/>
       <c r="CT32" t="inlineStr"/>
-      <c r="CU32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -7142,7 +7106,6 @@
       <c r="CR33" t="inlineStr"/>
       <c r="CS33" t="inlineStr"/>
       <c r="CT33" t="inlineStr"/>
-      <c r="CU33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -7435,7 +7398,6 @@
       <c r="CR34" t="inlineStr"/>
       <c r="CS34" t="inlineStr"/>
       <c r="CT34" t="inlineStr"/>
-      <c r="CU34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -7704,7 +7666,6 @@
       <c r="CR35" t="inlineStr"/>
       <c r="CS35" t="inlineStr"/>
       <c r="CT35" t="inlineStr"/>
-      <c r="CU35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -7847,8 +7808,8 @@
       </c>
       <c r="AM36" t="inlineStr">
         <is>
-          <t>Overall: 19 7/16 x 13 x 9 1/4 in. (49.4 x 33 x 23.5 cm); 352 oz. 18 dwt. (10977 g)
-Body: H. 18 7/8 in. (47.9 cm)
+          <t>Overall: 19 7/16 x 13 x 9 1/4 in. (49.4 x 33 x 23.5 cm); 352 oz. 18 dwt. (10977 g)
+Body: H. 18 7/8 in. (47.9 cm)
 Cover: 4 1/4 x 4 13/16 in. (10.8 x 12.2 cm); 19 oz. 6 dwt. (600.1 g)</t>
         </is>
       </c>
@@ -7924,17 +7885,11 @@
       <c r="BK36" t="inlineStr"/>
       <c r="BL36" t="inlineStr">
         <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="BM36" t="inlineStr">
-        <is>
-          <t>Cover</t>
-        </is>
-      </c>
-      <c r="BN36" t="n">
-        <v>12.2238</v>
-      </c>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="BM36" t="inlineStr"/>
+      <c r="BN36" t="inlineStr"/>
       <c r="BO36" t="inlineStr">
         <is>
           <t>Birds</t>
@@ -7980,11 +7935,15 @@
           <t>https://www.wikidata.org/wiki/Q729</t>
         </is>
       </c>
-      <c r="BX36" t="inlineStr"/>
+      <c r="BX36" t="n">
+        <v>23.495</v>
+      </c>
       <c r="BY36" t="n">
-        <v>10.795</v>
-      </c>
-      <c r="BZ36" t="inlineStr"/>
+        <v>49.3713</v>
+      </c>
+      <c r="BZ36" t="n">
+        <v>33</v>
+      </c>
       <c r="CA36" t="n">
         <v>162539</v>
       </c>
@@ -8010,56 +7969,57 @@
       </c>
       <c r="CF36" t="inlineStr"/>
       <c r="CG36" t="n">
+        <v>10.977</v>
+      </c>
+      <c r="CH36" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="CI36" t="inlineStr">
+        <is>
+          <t>Cover</t>
+        </is>
+      </c>
+      <c r="CJ36" t="n">
+        <v>12.2238</v>
+      </c>
+      <c r="CK36" t="n">
+        <v>10.795</v>
+      </c>
+      <c r="CL36" t="n">
         <v>0.6001</v>
       </c>
-      <c r="CH36" t="inlineStr">
+      <c r="CM36" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="CI36" t="inlineStr">
+      <c r="CN36" t="inlineStr">
         <is>
           <t>Body</t>
         </is>
       </c>
-      <c r="CJ36" t="n">
+      <c r="CO36" t="n">
         <v>47.9426</v>
       </c>
-      <c r="CK36" t="inlineStr">
-        <is>
-          <t>Overall</t>
-        </is>
-      </c>
-      <c r="CL36" t="inlineStr"/>
-      <c r="CM36" t="n">
-        <v>23.495</v>
-      </c>
-      <c r="CN36" t="n">
-        <v>49.3713</v>
-      </c>
-      <c r="CO36" t="n">
-        <v>10.977</v>
-      </c>
-      <c r="CP36" t="n">
-        <v>33</v>
+      <c r="CP36" t="inlineStr">
+        <is>
+          <t>Garlands</t>
+        </is>
       </c>
       <c r="CQ36" t="inlineStr">
         <is>
-          <t>Garlands</t>
+          <t>http://vocab.getty.edu/page/aat/300167386</t>
         </is>
       </c>
       <c r="CR36" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/aat/300167386</t>
-        </is>
-      </c>
-      <c r="CS36" t="inlineStr">
-        <is>
           <t>https://www.wikidata.org/wiki/Q756600</t>
         </is>
       </c>
+      <c r="CS36" t="inlineStr"/>
       <c r="CT36" t="inlineStr"/>
-      <c r="CU36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -8296,7 +8256,6 @@
       <c r="CR37" t="inlineStr"/>
       <c r="CS37" t="inlineStr"/>
       <c r="CT37" t="inlineStr"/>
-      <c r="CU37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -8575,13 +8534,12 @@
       <c r="CP38" t="inlineStr"/>
       <c r="CQ38" t="inlineStr"/>
       <c r="CR38" t="inlineStr"/>
-      <c r="CS38" t="inlineStr"/>
+      <c r="CS38" t="inlineStr">
+        <is>
+          <t>https://images.metmuseum.org/CRDImages/ad/original/DP247756.jpg</t>
+        </is>
+      </c>
       <c r="CT38" t="inlineStr">
-        <is>
-          <t>https://images.metmuseum.org/CRDImages/ad/original/DP247756.jpg</t>
-        </is>
-      </c>
-      <c r="CU38" t="inlineStr">
         <is>
           <t>https://images.metmuseum.org/CRDImages/ad/original/117430.jpg</t>
         </is>
@@ -8861,28 +8819,27 @@
       <c r="CM39" t="inlineStr"/>
       <c r="CN39" t="inlineStr"/>
       <c r="CO39" t="inlineStr"/>
-      <c r="CP39" t="inlineStr"/>
+      <c r="CP39" t="inlineStr">
+        <is>
+          <t>Admirals</t>
+        </is>
+      </c>
       <c r="CQ39" t="inlineStr">
         <is>
-          <t>Admirals</t>
+          <t>http://vocab.getty.edu/page/aat/300236014</t>
         </is>
       </c>
       <c r="CR39" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/aat/300236014</t>
+          <t>https://www.wikidata.org/wiki/Q132851</t>
         </is>
       </c>
       <c r="CS39" t="inlineStr">
         <is>
-          <t>https://www.wikidata.org/wiki/Q132851</t>
-        </is>
-      </c>
-      <c r="CT39" t="inlineStr">
-        <is>
           <t>https://images.metmuseum.org/CRDImages/ad/original/DP247755.jpg</t>
         </is>
       </c>
-      <c r="CU39" t="inlineStr"/>
+      <c r="CT39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -9099,7 +9056,6 @@
       <c r="CR40" t="inlineStr"/>
       <c r="CS40" t="inlineStr"/>
       <c r="CT40" t="inlineStr"/>
-      <c r="CU40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -9358,9 +9314,8 @@
       <c r="CR41" t="inlineStr"/>
       <c r="CS41" t="inlineStr"/>
       <c r="CT41" t="inlineStr"/>
-      <c r="CU41" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>